<commit_message>
automation API poc changes & INS complete regression suite 23 scripts
</commit_message>
<xml_diff>
--- a/InputFiles/INS/TC01_INS_CancerType-BladderCancer.xlsx
+++ b/InputFiles/INS/TC01_INS_CancerType-BladderCancer.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-07-15-2024/Commons_Automation/InputFiles/INS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/radhakrishnang2/Desktop/Automation/Sep2024/Commons_Automation/InputFiles/INS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1C0100-0811-EE43-A227-CEF0FAA5A456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC9DC8C-BC96-8C46-8077-45359873EDDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="-1380" windowWidth="51200" windowHeight="28800" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17440" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -85,51 +85,7 @@
 LEFT JOIN 
     df_publication pub ON prj.project_id = pub."project.project_id"
 WHERE 
-    prg.cancer_type IN ('Bladder Cancer');</t>
-  </si>
-  <si>
-    <t>SELECT DISTINCT
-    prj.project_id AS "Project ID", 
-    prj.project_title AS "Project Title",
-    prj.org_name AS "Organization",
-    prj.project_start_date AS "Project Start Date",
-    prj.project_end_date AS "Project End Date"
-FROM 
-    df_project prj
-LEFT JOIN 
-    df_program prg ON prj."program.program_id" = prg.program_id
-LEFT JOIN 
-    df_grant gnt ON prj.project_id = gnt."project.project_id"
-LEFT JOIN 
-    df_publication pub ON prj.project_id = pub."project.project_id"
-WHERE 
-     prg.cancer_type IN ('Bladder Cancer')
-ORDER BY 
-    prj.project_id ASC
-LIMIT 100;</t>
-  </si>
-  <si>
-    <t>SELECT DISTINCT
-    gnt.grant_id AS "Grant ID", 
-    prj.project_id AS "Project",
-    gnt.grant_title AS "Grant Title",
-    gnt.principal_investigators AS "Principal Investigators",
-    gnt.program_officers AS "Program Officers",
-    gnt.fiscal_year AS "Fiscal Year",
-    gnt.project_end_date AS "Project End Date"
-FROM 
-    df_grant gnt
-LEFT JOIN 
-    df_project prj ON gnt."project.project_id" = prj.project_id
-LEFT JOIN 
-    df_program prg ON prj."program.program_id" = prg.program_id
-LEFT JOIN 
-    df_publication pub ON prj.project_id = pub."project.project_id"
-WHERE 
-    prg.cancer_type IN ('Bladder Cancer')
-ORDER BY 
-    gnt.grant_id ASC
-LIMIT 100;</t>
+    prg.cancer_type LIKE '%Bladder Cancer%'</t>
   </si>
   <si>
     <t>SELECT DISTINCT
@@ -153,7 +109,7 @@
 LEFT JOIN 
     df_grant gnt ON prj.project_id = gnt."project.project_id"
 WHERE 
-     prg.cancer_type IN ('Bladder Cancer')
+     prg.cancer_type LIKE '%Bladder Cancer%'
 ORDER BY 
     pub.pmid ASC
 LIMIT 100;</t>
@@ -161,19 +117,65 @@
   <si>
     <t>SELECT DISTINCT 
     prg.program_name AS "Program",
-    CASE 
-        WHEN prg.program_link = 'https://trp.cancer.gov/spores/abstracts/mskcc_bladder.htm' THEN 'SPORE in Bladder Cancer'        
+CASE
+    WHEN prg.program_link IS NOT NULL THEN prg.program_acronym
         ELSE prg.program_link
     END  AS "Website",
     prg.focus_area AS "Focus Area",
     prg.cancer_type AS "Cancer Type",
-    prg.data_link AS "Data Location Details"
+ CASE 
+        WHEN prg.data_link IS NOT NULL THEN prg.program_acronym     
+        ELSE prg.data_link
+    END AS "Data Location Details"
 FROM 
     df_program prg
+WHERE      prg.cancer_type LIKE '%Bladder Cancer%'
+ORDER BY 
+    lower(prg.program_name) ASC
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT
+    prj.project_id AS "Project ID", 
+    prj.project_title AS "Project Title",
+    prj.org_name AS "Organization",
+    prj.project_start_date AS "Project Start Date",
+    prj.project_end_date AS "Project End Date"
+FROM 
+    df_project prj
+LEFT JOIN 
+    df_program prg ON prj."program.program_id" = prg.program_id
+LEFT JOIN 
+    df_grant gnt ON prj.project_id = gnt."project.project_id"
+LEFT JOIN 
+    df_publication pub ON prj.project_id = pub."project.project_id"
 WHERE 
-     prg.cancer_type IN ('Bladder Cancer')
+     prg.cancer_type LIKE '%Bladder Cancer%'
 ORDER BY 
-    prg.program_name ASC
+    lower(prj.project_id) ASC
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT
+    gnt.grant_id AS "Grant ID", 
+    prj.project_id AS "Project",
+    gnt.grant_title AS "Grant Title",
+    gnt.principal_investigators AS "Principal Investigators",
+    gnt.program_officers AS "Program Officers",
+    gnt.fiscal_year AS "Fiscal Year",
+    gnt.project_end_date AS "Project End Date"
+FROM 
+    df_grant gnt
+LEFT JOIN 
+    df_project prj ON gnt."project.project_id" = prj.project_id
+LEFT JOIN 
+    df_program prg ON prj."program.program_id" = prg.program_id
+LEFT JOIN 
+    df_publication pub ON prj.project_id = pub."project.project_id"
+WHERE 
+    prg.cancer_type LIKE '%Bladder Cancer%'
+ORDER BY 
+    lower(gnt.grant_id) ASC
 LIMIT 100;</t>
   </si>
 </sst>
@@ -576,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -611,9 +613,9 @@
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D2" t="s">
@@ -628,15 +630,15 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="356" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>13</v>
+      <c r="B4" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -644,8 +646,8 @@
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
+      <c r="B5" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="C5" s="2"/>
     </row>

</xml_diff>

<commit_message>
corrected syntax issue for ins
</commit_message>
<xml_diff>
--- a/InputFiles/INS/TC01_INS_CancerType-BladderCancer.xlsx
+++ b/InputFiles/INS/TC01_INS_CancerType-BladderCancer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/radhakrishnang2/Desktop/Automation/Sep2024/Commons_Automation/InputFiles/INS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/radhakrishnang2/Desktop/Automation/gayathri26sep/Commons_Automation/InputFiles/INS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC9DC8C-BC96-8C46-8077-45359873EDDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E11DE5-FD23-2049-8671-68EFAD2D9066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17440" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -71,6 +71,26 @@
     <t>TC01_INS_CancerType-BladderCancer_WebData.xlsx</t>
   </si>
   <si>
+    <t>SELECT DISTINCT 
+    prg.program_name AS "Program",
+  CASE
+    WHEN prg.program_link IS NOT NULL THEN prg.program_acronym
+        ELSE prg.program_link
+    END  AS "Website",
+    prg.focus_area AS "Special Topic",
+    prg.cancer_type AS "Cancer Type",
+ CASE 
+        WHEN prg.data_link IS NOT NULL THEN prg.program_acronym     
+        ELSE prg.data_link
+    END AS "Data Location Details"FROM 
+    df_program prg
+WHERE 
+     prg.cancer_type LIKE '%Bladder Cancer%'
+ORDER BY 
+    lower(prg.program_name) ASC
+LIMIT 100;</t>
+  </si>
+  <si>
     <t>SELECT DISTINCT
     COUNT(DISTINCT prg.program_id) AS "Programs",
     COUNT(DISTINCT prj.project_id) AS "Projects",
@@ -85,60 +105,13 @@
 LEFT JOIN 
     df_publication pub ON prj.project_id = pub."project.project_id"
 WHERE 
-    prg.cancer_type LIKE '%Bladder Cancer%'</t>
-  </si>
-  <si>
-    <t>SELECT DISTINCT
-    pub.pmid AS "PubMed ID", 
-    pub.title AS "Title",
-    pub.authors AS "Authors",
-    pub.publication_date AS "Publication Date",
-    pub.cited_by AS "Cited By",
-    CASE 
-    WHEN pub.relative_citation_ratio = 0 THEN '0'
-    WHEN pub.relative_citation_ratio = 7.0 THEN '7'
-    WHEN pub.relative_citation_ratio = ROUND(pub.relative_citation_ratio) THEN CAST(ROUND(pub.relative_citation_ratio) AS VARCHAR) 
-    ELSE CAST(ROUND(pub.relative_citation_ratio, 2) AS VARCHAR)
-END AS "Relative Citation Ratio"
-FROM 
-    df_publication pub
-LEFT JOIN 
-    df_project prj ON pub."project.project_id" = prj.project_id
-LEFT JOIN 
-    df_program prg ON prj."program.program_id" = prg.program_id
-LEFT JOIN 
-    df_grant gnt ON prj.project_id = gnt."project.project_id"
-WHERE 
-     prg.cancer_type LIKE '%Bladder Cancer%'
-ORDER BY 
-    pub.pmid ASC
-LIMIT 100;</t>
-  </si>
-  <si>
-    <t>SELECT DISTINCT 
-    prg.program_name AS "Program",
-CASE
-    WHEN prg.program_link IS NOT NULL THEN prg.program_acronym
-        ELSE prg.program_link
-    END  AS "Website",
-    prg.focus_area AS "Focus Area",
-    prg.cancer_type AS "Cancer Type",
- CASE 
-        WHEN prg.data_link IS NOT NULL THEN prg.program_acronym     
-        ELSE prg.data_link
-    END AS "Data Location Details"
-FROM 
-    df_program prg
-WHERE      prg.cancer_type LIKE '%Bladder Cancer%'
-ORDER BY 
-    lower(prg.program_name) ASC
-LIMIT 100;</t>
+    prg.cancer_type LIKE '%Bladder Cancer%';</t>
   </si>
   <si>
     <t>SELECT DISTINCT
     prj.project_id AS "Project ID", 
     prj.project_title AS "Project Title",
-    prj.org_name AS "Organization",
+    prj.project_org_name AS "Organization",
     prj.project_start_date AS "Project Start Date",
     prj.project_end_date AS "Project End Date"
 FROM 
@@ -163,7 +136,7 @@
     gnt.principal_investigators AS "Principal Investigators",
     gnt.program_officers AS "Program Officers",
     gnt.fiscal_year AS "Fiscal Year",
-    gnt.project_end_date AS "Project End Date"
+    gnt.grant_end_date AS "Project End Date"
 FROM 
     df_grant gnt
 LEFT JOIN 
@@ -173,9 +146,38 @@
 LEFT JOIN 
     df_publication pub ON prj.project_id = pub."project.project_id"
 WHERE 
-    prg.cancer_type LIKE '%Bladder Cancer%'
+    prg.cancer_type  LIKE '%Bladder Cancer%'
 ORDER BY 
     lower(gnt.grant_id) ASC
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT
+    pub.pmid AS "PubMed ID", 
+    pub.publication_title AS "Title",
+    pub.authors AS "Authors",
+    pub.publication_date AS "Publication Date",
+    pub.cited_by AS "Cited By",
+    CASE 
+    WHEN pub.relative_citation_ratio = 0 THEN '0'
+    WHEN pub.relative_citation_ratio = 7.0 THEN '7'
+    WHEN pub.relative_citation_ratio = 2.0 THEN '2'
+  WHEN pub.relative_citation_ratio = 1.0 THEN '1'
+    WHEN pub.relative_citation_ratio = ROUND(pub.relative_citation_ratio) THEN CAST(ROUND(pub.relative_citation_ratio) AS VARCHAR) 
+    ELSE CAST(ROUND(pub.relative_citation_ratio, 2) AS VARCHAR)
+END AS "Relative Citation Ratio"
+FROM 
+    df_publication pub
+LEFT JOIN 
+    df_project prj ON pub."project.project_id" = prj.project_id
+LEFT JOIN 
+    df_program prg ON prj."program.program_id" = prg.program_id
+LEFT JOIN 
+    df_grant gnt ON prj.project_id = gnt."project.project_id"
+WHERE 
+     prg.cancer_type  LIKE '%Bladder Cancer%'
+ORDER BY 
+    lower(pub.pmid) ASC
 LIMIT 100;</t>
   </si>
 </sst>
@@ -183,23 +185,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -245,17 +233,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -579,7 +561,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -612,11 +594,11 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -629,16 +611,16 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>14</v>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="356" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>15</v>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -646,8 +628,8 @@
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>12</v>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -659,7 +641,7 @@
       <c r="C7" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>